<commit_message>
add test cases to excel
</commit_message>
<xml_diff>
--- a/documents/Test Cases.xlsx
+++ b/documents/Test Cases.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavier\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f50fb337da5a17b/University of Kansas/2023 Fall/Software Engineering I/Project/348_project/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F97D876-921B-40A2-A959-BD4B46C99518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2F97D876-921B-40A2-A959-BD4B46C99518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8799F902-3508-4873-9217-CB847DC5C447}"/>
   <bookViews>
     <workbookView xWindow="-24930" yWindow="1365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -48,75 +48,30 @@
     <t>TC01</t>
   </si>
   <si>
-    <t>Verification of basic addition calculations</t>
-  </si>
-  <si>
-    <t>20+21</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>TC02</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of basic subtraction calculations </t>
-  </si>
-  <si>
-    <t>40-14</t>
-  </si>
-  <si>
     <t>TC03</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of basic multiplication calculations </t>
-  </si>
-  <si>
-    <t>3*10</t>
-  </si>
-  <si>
     <t>TC04</t>
   </si>
   <si>
-    <t>Verification of basic division calculations</t>
-  </si>
-  <si>
-    <t>8 /2</t>
-  </si>
-  <si>
     <t>TC05</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of mixed operations calculations </t>
-  </si>
-  <si>
-    <t>8 / 2 * 3</t>
-  </si>
-  <si>
     <t>TC06</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of parentheses calculations </t>
-  </si>
-  <si>
-    <t>12 / (2*3)</t>
-  </si>
-  <si>
     <t>TC07</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of unary operations </t>
-  </si>
-  <si>
-    <t>10-(-5)</t>
-  </si>
-  <si>
     <t>TC08</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of floating point number calculations </t>
-  </si>
-  <si>
     <t>5*(3+7)-7/2</t>
   </si>
   <si>
@@ -126,22 +81,124 @@
     <t xml:space="preserve">Verification of complex mixed operations calculations </t>
   </si>
   <si>
-    <t>10.2+3.5</t>
-  </si>
-  <si>
     <t>TC10</t>
   </si>
   <si>
-    <t xml:space="preserve">Verification of invalid character errors </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 $ 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Character Error </t>
-  </si>
-  <si>
     <t>Tokenization error: Invalid character</t>
+  </si>
+  <si>
+    <t>20+2100</t>
+  </si>
+  <si>
+    <t>192-(123-2)</t>
+  </si>
+  <si>
+    <t>Subtraction with parenthesis</t>
+  </si>
+  <si>
+    <t>Basic addition</t>
+  </si>
+  <si>
+    <t>2^3+3-2^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exponentation </t>
+  </si>
+  <si>
+    <t>Mixed operators</t>
+  </si>
+  <si>
+    <t>10*(3-1)%7-1/2</t>
+  </si>
+  <si>
+    <t>Complex addition with extraneous parenthesis</t>
+  </si>
+  <si>
+    <t>((2+((2+2))))+((2-2))</t>
+  </si>
+  <si>
+    <t>Complex calculation with extraneous parenthesis</t>
+  </si>
+  <si>
+    <t>((10 - 2) - ((3 / 9) + ((42 % 3))))</t>
+  </si>
+  <si>
+    <t>Unary operations</t>
+  </si>
+  <si>
+    <t>10-(-5)+(+2)-(-3)</t>
+  </si>
+  <si>
+    <t>10.2+3.5-3.3^3</t>
+  </si>
+  <si>
+    <t>Floating point calculations with exponents</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>Unary operations with negative exponents</t>
+  </si>
+  <si>
+    <t>2-3^(-5)</t>
+  </si>
+  <si>
+    <t>+2-3^(-4-2)</t>
+  </si>
+  <si>
+    <t>Exponentiation with exponent operation</t>
+  </si>
+  <si>
+    <t>Unary negation with unary plus</t>
+  </si>
+  <si>
+    <t>((9 + 6)) / ((3 * 1) / (((2 + 2))) - 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zero division error checking </t>
+  </si>
+  <si>
+    <t>1+3+3+4*2+2/0</t>
+  </si>
+  <si>
+    <t>Divison by zero error</t>
+  </si>
+  <si>
+    <t>CALCULATOR ERROR: Divison by Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing parenthesis </t>
+  </si>
+  <si>
+    <t>(3+2-3</t>
+  </si>
+  <si>
+    <t>PARSER ERROR: Mismatched parenthesis</t>
+  </si>
+  <si>
+    <t>Invalid characters</t>
+  </si>
+  <si>
+    <t>7@2#4</t>
+  </si>
+  <si>
+    <t>Invalid characters error</t>
+  </si>
+  <si>
+    <t>Missing parenthesis error</t>
   </si>
 </sst>
 </file>
@@ -181,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
+      <alignment horizontal="right" vertical="center" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,18 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -504,170 +561,161 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>41</v>
-      </c>
-      <c r="E2">
-        <v>41</v>
+        <v>2120</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>26</v>
-      </c>
-      <c r="E3">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>7.6666666666700003</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>7.6666699999999999</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>13.7</v>
+        <v>-22.236999999999998</v>
       </c>
       <c r="E9">
-        <v>13.7</v>
+        <v>-22.236999999999998</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D10">
         <v>46.5</v>
@@ -676,30 +724,134 @@
         <v>46.5</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>1.9958847</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.9958800000000001</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>1.9986280000000001</v>
+      </c>
+      <c r="E12">
+        <v>1.9986299999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13">
+        <v>-60</v>
+      </c>
+      <c r="E13">
+        <v>-60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
-        <v>9</v>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1" xr:uid="{5A6D5FA3-FF02-4046-88D1-152481F6DCAA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>